<commit_message>
Manuscript revisions and response to reviewers; seedling plot analysis and figures in response to reviewers (round 2)
</commit_message>
<xml_diff>
--- a/Figures and Graphs/Seedling plot descriptions.xlsx
+++ b/Figures and Graphs/Seedling plot descriptions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="69">
   <si>
     <t>Site</t>
   </si>
@@ -102,9 +103,6 @@
   </si>
   <si>
     <t>10-13m</t>
-  </si>
-  <si>
-    <t>10-18m</t>
   </si>
   <si>
     <t>Ochrosia oppositifolia, Cycas micronesica, Macaranga thompsonii</t>
@@ -205,6 +203,15 @@
     <t>Eugenia reinwardtiana, Aglaia mariannensis</t>
   </si>
   <si>
+    <t>Mammea odorata, Aglaia mariannensis, Meiogyne cylindrocarpa, Ochrosia oppositifolia</t>
+  </si>
+  <si>
+    <t>Mammea odorata, Ochrosia oppositifolia, Cycas micronesica, Meiogyne cylindrocarpa</t>
+  </si>
+  <si>
+    <r>
+      <t>8-12m (</t>
+    </r>
     <r>
       <rPr>
         <i/>
@@ -214,7 +221,77 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Ochrosia oppositifolia, Meiogyne cylindrocarpa, Carica papaya</t>
+      <t>Cycas micronesica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3m)</t>
+    </r>
+  </si>
+  <si>
+    <t>Few large, 50-cm-high boulders, &lt;20% exposed red soil, mostly 5-10cm-diameter rocks</t>
+  </si>
+  <si>
+    <t>Mostly 5-10cm-diameter rocks with few large, 50-cm-high boulders, &lt;20% exposed red soil</t>
+  </si>
+  <si>
+    <t>Mostly flat with scattered limestone rocks 10-20 cm in diameter, mixed leaf litter</t>
+  </si>
+  <si>
+    <t>flat</t>
+  </si>
+  <si>
+    <t>slight downward slope (&lt;5 degrees) towards east</t>
+  </si>
+  <si>
+    <t>60% of ground cover is large rocks &gt;20cm in diameter, some (~20% substrate) exposed red dirt</t>
+  </si>
+  <si>
+    <t>very rocky, loose rocks 10-50cm in diameter, small amounts (~10-15%) of exposed red dirt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">very rocky, high amount of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eugenia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> leaf litter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ochrosia oppositifolia, Meiogyne cylindrocarpa, (Carica papaya)</t>
     </r>
     <r>
       <rPr>
@@ -249,14 +326,34 @@
     </r>
   </si>
   <si>
-    <t>Mammea odorata, Aglaia mariannensis, Meiogyne cylindrocarpa, Ochrosia oppositifolia</t>
-  </si>
-  <si>
-    <t>Mammea odorata, Ochrosia oppositifolia, Cycas micronesica, Meiogyne cylindrocarpa</t>
-  </si>
-  <si>
-    <r>
-      <t>8-12m (</t>
+    <r>
+      <t>10-18m, (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Cycas micronesica </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3m)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9-15m, </t>
     </r>
     <r>
       <rPr>
@@ -277,55 +374,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 3m)</t>
-    </r>
-  </si>
-  <si>
-    <t>Few large, 50-cm-high boulders, &lt;20% exposed red soil, mostly 5-10cm-diameter rocks</t>
-  </si>
-  <si>
-    <t>Mostly 5-10cm-diameter rocks with few large, 50-cm-high boulders, &lt;20% exposed red soil</t>
-  </si>
-  <si>
-    <t>Mostly flat with scattered limestone rocks 10-20 cm in diameter, mixed leaf litter</t>
-  </si>
-  <si>
-    <t>flat</t>
-  </si>
-  <si>
-    <t>slight downward slope (&lt;5 degrees) towards east</t>
-  </si>
-  <si>
-    <t>60% of ground cover is large rocks &gt;20cm in diameter, some (~20% substrate) exposed red dirt</t>
-  </si>
-  <si>
-    <t>very rocky, loose rocks 10-50cm in diameter, small amounts (~10-15%) of exposed red dirt</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">very rocky, high amount of </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Eugenia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> leaf litter</t>
-    </r>
+      <t xml:space="preserve"> &lt;3m</t>
+    </r>
+  </si>
+  <si>
+    <t>adult trees</t>
+  </si>
+  <si>
+    <t>avg dbh</t>
+  </si>
+  <si>
+    <t>canopy cover</t>
+  </si>
+  <si>
+    <t>canopy height</t>
   </si>
 </sst>
 </file>
@@ -749,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -779,10 +841,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -830,7 +892,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -853,10 +915,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -868,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -901,10 +963,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -913,10 +975,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -927,10 +989,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -978,7 +1040,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -987,10 +1049,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -1001,10 +1063,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -1013,10 +1075,10 @@
         <v>8</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1049,10 +1111,10 @@
         <v>4</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -1061,10 +1123,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -1075,10 +1137,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -1087,10 +1149,10 @@
         <v>8</v>
       </c>
       <c r="C27" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1110,10 +1172,10 @@
       <c r="B29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="8">
         <v>0.85</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="8">
         <v>0.82</v>
       </c>
     </row>
@@ -1123,10 +1185,10 @@
         <v>4</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -1135,10 +1197,10 @@
         <v>5</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -1149,10 +1211,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -1176,7 +1238,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -1197,10 +1259,10 @@
         <v>4</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -1209,10 +1271,10 @@
         <v>5</v>
       </c>
       <c r="C37" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -1247,10 +1309,10 @@
         <v>2</v>
       </c>
       <c r="C40" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1297,10 +1359,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1345,10 +1407,10 @@
         <v>4</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -1357,7 +1419,7 @@
         <v>5</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>20</v>
@@ -1367,4 +1429,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>